<commit_message>
bez pracy nie ma kolaczy
</commit_message>
<xml_diff>
--- a/zadanie3/faktury-sprzedazowe-test.xlsx
+++ b/zadanie3/faktury-sprzedazowe-test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FiFi\PZ1\zadanie3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{E5A09D8B-DE72-4A73-A733-880180B25643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D92908F-FB8F-4933-A75E-D3B1860B3E9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-15870" yWindow="270" windowWidth="15990" windowHeight="24840"/>
   </bookViews>
   <sheets>
     <sheet name="faktury-sprzedazowe-test" sheetId="1" r:id="rId1"/>
@@ -20,63 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="284">
-  <si>
-    <t xml:space="preserve">	2	1Â 000,00 zĹ‚	23	460,00 zĹ‚	2Â 000,00 zĹ‚	2Â 460,00 zĹ‚	85Â 833,75 zĹ‚	105Â 575,51 zĹ‚
-Firma1 Sp. z o.o	AL. A. Mickiewicza 141, 31-127 KrakĂłw	113-29-95-753 	2020-11-25	2020-11-25	3-25/11/2020	Prace rozwojowe - #50956 : Grupowanie pojazdĂłw - rozliczenie czÄ™Ĺ›Ä‡ 2	29,2125	1Â 000,00 zĹ‚	23	6Â 718,88 zĹ‚	29Â 212,50 zĹ‚	35Â 931,38 zĹ‚	85Â 833,75 zĹ‚	105Â 575,51 zĹ‚
-Firma1 Sp. z o.o	AL. A. Mickiewicza 141, 31-127 KrakĂłw	113-29-95-753 	2020-11-25	2020-11-25	3-25/11/2020	Prace rozwojowe - #60386 : ObsĹ‚uga pojazdĂłw importowanych â€“ rozliczenie czÄ™Ĺ›Ä‡ 2	30,87125	1Â 000,00 zĹ‚	23	7Â 100,39 zĹ‚	30Â 871,25 zĹ‚	37Â 971,64 zĹ‚	85Â 833,75 zĹ‚	105Â 575,51 zĹ‚
-Firma9 SP. Z O.O.	ul. Dobra 28, 00-344 Warszawa	118-16-48-603	2020-12-07	2020-11-30	1-07/12/2020	NAJEM SERWERA ZA OKRES 11.2020 (SPECYFIKACJA ZGODNA Z UMOWÄ„)   	1	13Â 000,00 zĹ‚	23	2Â 990,00 zĹ‚	13Â 000,00 zĹ‚	15Â 990,00 zĹ‚	13Â 000,00 zĹ‚	15Â 990,00 zĹ‚
-Firma8 Sp. z o.o. sp.k.	ul. Krkusowa 12, 30-123 KrakĂłw	677-00-46-633	2020-12-07	2020-11-30	2-07/12/2020	Firma8 - prace projektowe oraz programistyczne, zgodnie z zaĹ‚Ä…cznikiem	12,46875	1Â 250,00 zĹ‚	23	3Â 584,77 zĹ‚	15Â 585,94 zĹ‚	19Â 170,71 zĹ‚	15Â 585,94 zĹ‚	19Â 170,71 zĹ‚
-Firma4	ul. MICKIEWICZA 1/5, 33-100 TARNĂ“W	873-171-75-73	2020-12-07	2020-11-30	3-07/12/2020	Abonament â€“ aktywne karty SIM zgodnie z zaĹ‚Ä…cznikiem 	536,86620	7,50 zĹ‚	23	926,10 zĹ‚	4Â 026,50 zĹ‚	4Â 952,60 zĹ‚	4Â 026,50 zĹ‚	4Â 952,60 zĹ‚
-Firma4	ul. MICKIEWICZA 1/5, 33-100 TARNĂ“W	873-171-75-73	2020-12-07	2020-11-30	4-07/12/2020	UrzÄ…dzenia GPS â€“ terminale/montaĹĽ â€“ listopad 2020 zgodnie z zaĹ‚Ä…cznikiem 	52	280,00 zĹ‚	23	3Â 348,80 zĹ‚	14Â 560,00 zĹ‚	17Â 908,80 zĹ‚	14Â 560,00 zĹ‚	17Â 908,80 zĹ‚
-Firma4	ul. MICKIEWICZA 1/5, 33-100 TARNĂ“W	873-171-75-73	2020-12-07	2020-11-30	5-07/12/2020	UrzÄ…dzenia GPS â€“ terminale - uzupeĹ‚nienie stocka urzÄ…dzeĹ„	100	280,00 zĹ‚	23	6Â 440,00 zĹ‚	28Â 000,00 zĹ‚	34Â 440,00 zĹ‚	28Â 000,00 zĹ‚	34Â 440,00 zĹ‚
-Firma3 sp. z o.o.	ul. Krkusowa 12, 30-123 KrakĂłw	675-152-93-71	2020-12-07	2020-11-30	6-07/12/2020	ZarzÄ…dzanie infrastrukturÄ… serwerowÄ… oraz usĹ‚ugami dla projektu Innovative- ZGODNIE Z RAPORTEM	1	3Â 090,63 zĹ‚	23	710,84 zĹ‚	3Â 090,63 zĹ‚	3Â 801,47 zĹ‚	3Â 090,63 zĹ‚	3Â 801,47 zĹ‚
-Firma3 sp. z o.o.	ul. Krkusowa 12, 30-123 KrakĂłw	675-152-93-71	2020-12-09	2020-11-30	1-09/12/2020	Firma3 - prace projektowe oraz programistyczne zwiÄ…zane z rozwojem, zgodne z zaĹ‚Ä…cznikiem	78,8000	1Â 250,00 zĹ‚	23	21Â 505,00 zĹ‚	93Â 500,00 zĹ‚	115Â 005,00 zĹ‚	106Â 340,00 zĹ‚	130Â 798,20 zĹ‚
-Firma3 sp. z o.o.	ul. Krkusowa 12, 30-123 KrakĂłw	675-152-93-71	2020-12-09	2020-11-30	1-09/12/2020	ZarzÄ…dzanie infrastrukturÄ… serwerowÄ… oraz usĹ‚ugami dla projektu Firma3 â€“ Premium	1	7Â 840,00 zĹ‚	23	1Â 803,20 zĹ‚	7Â 840,00 zĹ‚	9Â 643,20 zĹ‚	106Â 340,00 zĹ‚	130Â 798,20 zĹ‚
-Firma3 sp. z o.o.	ul. Krkusowa 12, 30-123 KrakĂłw	675-152-93-71	2020-12-09	2020-11-30	1-09/12/2020	Firma3 - prace projektowe oraz programistyczne zwiÄ…zane z utrzymaniem i poprawÄ… bĹ‚Ä™dĂłw oraz bieĹĽÄ…cymi dziaĹ‚aniami,  zgodne z zaĹ‚Ä…cznikiem	4	1Â 250,00 zĹ‚	23	1Â 150,00 zĹ‚	5Â 000,00 zĹ‚	6Â 150,00 zĹ‚	106Â 340,00 zĹ‚	130Â 798,20 zĹ‚
-Firma3 sp. z o.o.	ul. Krkusowa 12, 30-123 KrakĂłw	675-152-93-71	2020-12-09	2020-11-30	2-09/12/2020	Innovative - prace projektowe oraz programistyczne zwiÄ…zane z rozwojem, zgodnie z zaĹ‚Ä…cznikiem	4,71875	1Â 250,00 zĹ‚	23	1Â 356,64 zĹ‚	5Â 898,44 zĹ‚	7Â 255,08 zĹ‚	7Â 070,32 zĹ‚	8Â 696,49 zĹ‚
-Firma3 sp. z o.o.	ul. Krkusowa 12, 30-123 KrakĂłw	675-152-93-71	2020-12-09	2020-11-30	2-09/12/2020	Innovative - prace projektowe oraz programistyczne zwiÄ…zane z utrzymaniem i poprawÄ… bĹ‚Ä™dĂłw oraz bieĹĽÄ…cymi dziaĹ‚aniami,  zgodnie z zaĹ‚Ä…cznikiem	0,93750	1Â 250,00 zĹ‚	23	269,53 zĹ‚	1Â 171,88 zĹ‚	1Â 441,41 zĹ‚	7Â 070,32 zĹ‚	8Â 696,49 zĹ‚
-Firma5 SP. Z O.O.	UL. FELIKSA RADWAĹSKIEGO 15/1, 30-065 KRAKĂ“W	634-27-26-447	2020-12-10	2020-12-10	1-10/12/2020	Czynsz z tytuĹ‚u najmu powierzchni w budynku przy ul. RadwaĹ„skiego 15 w Krakowie za GrudzieĹ„ 2020	1	3Â 000,00 zĹ‚	23	690,00 zĹ‚	3Â 000,00 zĹ‚	3Â 690,00 zĹ‚	3Â 000,00 zĹ‚	3Â 690,00 zĹ‚
-Firma6 SP. Z O.O.	UL. FELIKSA RADWAĹSKIEGO 15/1, 30-065 KRAKĂ“W	676-247-94-12	2020-12-10	2020-12-10	2-10/12/2020	Czynsz z tytuĹ‚u najmu powierzchni w budynku przy ul. RadwaĹ„skiego 15 w Krakowie za GrudzieĹ„ 2020	1	7Â 000,00 zĹ‚	23	1Â 610,00 zĹ‚	7Â 000,00 zĹ‚	8Â 610,00 zĹ‚	7Â 000,00 zĹ‚	8Â 610,00 zĹ‚
-Firma1 Sp. z o.o	AL. A. Mickiewicza 141, 31-127 KrakĂłw	113-29-95-753 	2020-12-14	2020-11-30	1-14/12/2020	Prace zwiÄ…zane z utrzymaniem aplikacji Aplikacja sprzedaĹĽowa w listopadzie 2020, zgodnie z zaĹ‚Ä…cznikiem	3,97500	1Â 000,00 zĹ‚	23	914,25 zĹ‚	3Â 975,00 zĹ‚	4Â 889,25 zĹ‚	28Â 920,00 zĹ‚	35Â 571,60 zĹ‚
-Firma1 Sp. z o.o	AL. A. Mickiewicza 141, 31-127 KrakĂłw	113-29-95-753 	2020-12-14	2020-11-30	1-14/12/2020	Prace zwiÄ…zane z utrzymaniem aplikacji Sellcar w listopadzie 2020, zgodnie z zaĹ‚Ä…cznikiem	16,06625	1Â 000,00 zĹ‚	23	3Â 695,24 zĹ‚	16Â 066,25 zĹ‚	19Â 761,49 zĹ‚	28Â 920,00 zĹ‚	35Â 571,60 zĹ‚
-Firma1 Sp. z o.o	AL. A. Mickiewicza 141, 31-127 KrakĂłw	113-29-95-753 	2020-12-14	2020-11-30	1-14/12/2020	Prace zwiÄ…zane z utrzymaniem systemu Aplikacja GPS w listopadzie 2020, zgodnie z zaĹ‚Ä…cznikiem	5,69375	1Â 000,00 zĹ‚	23	1Â 309,56 zĹ‚	5Â 693,75 zĹ‚	7Â 003,31 zĹ‚	28Â 920,00 zĹ‚	35Â 571,60 zĹ‚
-Firma1 Sp. z o.o	AL. A. Mickiewicza 141, 31-127 KrakĂłw	113-29-95-753 	2020-12-14	2020-11-30	1-14/12/2020	Prace zwiÄ…zane z utrzymaniem systemu Aplikacja ubezpieczeniowa w listopadzie 2020, zgodnie z zaĹ‚Ä…cznikiem	0,50000	1Â 000,00 zĹ‚	23	115,00 zĹ‚	500,00 zĹ‚	615,00 zĹ‚	28Â 920,00 zĹ‚	35Â 571,60 zĹ‚
-Firma1 Sp. z o.o	AL. A. Mickiewicza 141, 31-127 KrakĂłw	113-29-95-753 	2020-12-14	2020-11-30	1-14/12/2020	Prace zwiÄ…zane z utrzymaniem systemu Aplikacja windykacyjna w listopadzie 2020, zgodnie z zaĹ‚Ä…cznikiem	0,43750	1Â 000,00 zĹ‚	23	100,63 zĹ‚	437,50 zĹ‚	538,13 zĹ‚	28Â 920,00 zĹ‚	35Â 571,60 zĹ‚
-Firma1 Sp. z o.o	AL. A. Mickiewicza 141, 31-127 KrakĂłw	113-29-95-753 	2020-12-14	2020-11-30	1-14/12/2020	Prace zwiÄ…zane z utrzymaniem systemu Ces w listopadzie 2020, zgodnie z zaĹ‚Ä…cznikiem	0,53125	1Â 000,00 zĹ‚	23	122,19 zĹ‚	531,25 zĹ‚	653,44 zĹ‚	28Â 920,00 zĹ‚	35Â 571,60 zĹ‚
-Firma1 Sp. z o.o	AL. A. Mickiewicza 141, 31-127 KrakĂłw	113-29-95-753 	2020-12-14	2020-11-30	1-14/12/2020	Prace zwiÄ…zane z utrzymaniem usĹ‚ugi eFaktura w listopadzie 2020, zgodnie z zaĹ‚Ä…cznikiem	0,03125	1Â 000,00 zĹ‚	23	7,19 zĹ‚	31,25 zĹ‚	38,44 zĹ‚	28Â 920,00 zĹ‚	35Â 571,60 zĹ‚
-Firma1 Sp. z o.o	AL. A. Mickiewicza 141, 31-127 KrakĂłw	113-29-95-753 	2020-12-14	2020-11-30	1-14/12/2020	Prace zwiÄ…zane z utrzymaniem systemu Seyo (Portal Klienta) w listopadzie 2020, zgodnie z zaĹ‚Ä…cznikiem	0,12500	1Â 000,00 zĹ‚	23	28,75 zĹ‚	125,00 zĹ‚	153,75 zĹ‚	28Â 920,00 zĹ‚	35Â 571,60 zĹ‚
-Firma1 Sp. z o.o	AL. A. Mickiewicza 141, 31-127 KrakĂłw	113-29-95-753 	2020-12-14	2020-11-30	1-14/12/2020	Prace zwiÄ…zane z utrzymaniem â€“ wyceny w listopadzie 2020, zgodnie z zaĹ‚Ä…cznikiem	1,56000	1Â 000,00 zĹ‚	23	358,80 zĹ‚	1Â 560,00 zĹ‚	1Â 918,80 zĹ‚	28Â 920,00 zĹ‚	35Â 571,60 zĹ‚
-Firma1 Sp. z o.o	AL. A. Mickiewicza 141, 31-127 KrakĂłw	113-29-95-753 	2020-12-14	2020-11-30	2-14/12/2020	Prace zwiÄ…zane z utrzymaniem infrastruktury w listopadzie 2020, zgodnie z zaĹ‚Ä…cznikiem	13,54375	1Â 000,00 zĹ‚	23	3Â 115,06 zĹ‚	13Â 543,75 zĹ‚	16Â 658,81 zĹ‚	13Â 543,75 zĹ‚	16Â 658,81 zĹ‚
-Firma1 Sp. z o.o	AL. A. Mickiewicza 141, 31-127 KrakĂłw	113-29-95-753 	2020-12-14	2020-12-14	3-14/12/2020	Prace rozwojowe - #70418: SSR	19	1Â 000,00 zĹ‚	23	4Â 370,00 zĹ‚	19Â 000,00 zĹ‚	23Â 370,00 zĹ‚	45Â 093,75 zĹ‚	55Â 465,31 zĹ‚
-Firma1 Sp. z o.o	AL. A. Mickiewicza 141, 31-127 KrakĂłw	113-29-95-753 	2020-12-14	2020-12-14	3-14/12/2020	Prace rozwojowe - #70713: Wszystkie samochody razem i wartoĹ›Ä‡ na kaflu (ograniczony zakres)	15	1Â 000,00 zĹ‚	23	3Â 450,00 zĹ‚	15Â 000,00 zĹ‚	18Â 450,00 zĹ‚	45Â 093,75 zĹ‚	55Â 465,31 zĹ‚
-Firma1 Sp. z o.o	AL. A. Mickiewicza 141, 31-127 KrakĂłw	113-29-95-753 	2020-12-14	2020-12-14	3-14/12/2020	Prace rozwojowe - #70991: Finansowanie obce	4,75	1Â 000,00 zĹ‚	23	1Â 092,50 zĹ‚	4Â 750,00 zĹ‚	5Â 842,50 zĹ‚	45Â 093,75 zĹ‚	55Â 465,31 zĹ‚
-Firma1 Sp. z o.o	AL. A. Mickiewicza 141, 31-127 KrakĂłw	113-29-95-753 	2020-12-14	2020-12-14	3-14/12/2020	Prace rozwojowe - #69512: Raport danych klienta na podstawie danych z BIK	3,46875	1Â 000,00 zĹ‚	23	797,81 zĹ‚	3Â 468,75 zĹ‚	4Â 266,56 zĹ‚	45Â 093,75 zĹ‚	55Â 465,31 zĹ‚
-Firma1 Sp. z o.o	AL. A. Mickiewicza 141, 31-127 KrakĂłw	113-29-95-753 	2020-12-14	2020-12-14	3-14/12/2020	Prace rozwojowe - #70916: Zmiana kwoty minimalnej w zaleznoĹ›ci od przeznaczenia gotĂłwki	1	1Â 000,00 zĹ‚	23	230,00 zĹ‚	1Â 000,00 zĹ‚	1Â 230,00 zĹ‚	45Â 093,75 zĹ‚	55Â 465,31 zĹ‚
-Firma1 Sp. z o.o	AL. A. Mickiewicza 141, 31-127 KrakĂłw	113-29-95-753 	2020-12-14	2020-12-14	3-14/12/2020	Prace rozwojowe - #71459: SME	1,875	1Â 000,00 zĹ‚	23	431,25 zĹ‚	1Â 875,00 zĹ‚	2Â 306,25 zĹ‚	45Â 093,75 zĹ‚	55Â 465,31 zĹ‚
-Firma7 S.A.	ul. PostÄ™pu 18B, 02- 676 Warszawa	 531 30 92 922	2020-12-14	2020-12-14	4-14/12/2020	System â€žTankuj korzysĚciâ€ť zgodnie ze ZLECENIEM NR 5 z dnia 15.01.2020 â€“ rozliczenie rozszerzeĹ„, zgodnie z zaĹ‚Ä…cznikiem	41,60	1Â 400,00 zĹ‚	23	13Â 395,20 zĹ‚	58Â 240,00 zĹ‚	71Â 635,20 zĹ‚	58Â 240,00 zĹ‚	71Â 635,20 zĹ‚
-Firma3 sp. z o.o.	ul. Krkusowa 12, 30-123 KrakĂłw	675-152-93-71	2021-01-04	2020-12-30	1-04/01/2021	Innovative - prace projektowe oraz programistyczne zwiÄ…zane z rozwojem, zgodnie z zaĹ‚Ä…cznikiem	14,65625	1Â 250,00 zĹ‚	23	4Â 213,67 zĹ‚	18Â 320,31 zĹ‚	22Â 533,98 zĹ‚	19Â 414,06 zĹ‚	23Â 879,29 zĹ‚
-Firma3 sp. z o.o.	ul. Krkusowa 12, 30-123 KrakĂłw	675-152-93-71	2021-01-04	2020-12-30	1-04/01/2021	Innovative - prace projektowe oraz programistyczne zwiÄ…zane z utrzymaniem i poprawÄ… bĹ‚Ä™dĂłw oraz bieĹĽÄ…cymi dziaĹ‚aniami,  zgodnie z zaĹ‚Ä…cznikiem	0,87500	1Â 250,00 zĹ‚	23	251,56 zĹ‚	1Â 093,75 zĹ‚	1Â 345,31 zĹ‚	19Â 414,06 zĹ‚	23Â 879,29 zĹ‚
-Firma3 sp. z o.o.	ul. Krkusowa 12, 30-123 KrakĂłw	675-152-93-71	2021-01-04	2020-12-30	2-04/01/2021	ZarzÄ…dzanie infrastrukturÄ… serwerowÄ… oraz usĹ‚ugami dla projektu Innovative- ZGODNIE Z RAPORTEM	1	6Â 200,00 zĹ‚	23	1Â 426,00 zĹ‚	6Â 200,00 zĹ‚	7Â 626,00 zĹ‚	6Â 200,00 zĹ‚	7Â 626,00 zĹ‚
-Firma3 sp. z o.o.	ul. Krkusowa 12, 30-123 KrakĂłw	675-152-93-71	2021-01-04	2020-12-30	3-04/01/2021	Firma3 - prace projektowe oraz programistyczne zwiÄ…zane z rozwojem, zgodne z zaĹ‚Ä…cznikiem	95,26250	1Â 250,00 zĹ‚	23	26Â 237,97 zĹ‚	114Â 078,13 zĹ‚	140Â 316,10 zĹ‚	126Â 918,13 zĹ‚	156Â 109,30 zĹ‚
-Firma3 sp. z o.o.	ul. Krkusowa 12, 30-123 KrakĂłw	675-152-93-71	2021-01-04	2020-12-30	3-04/01/2021	ZarzÄ…dzanie infrastrukturÄ… serwerowÄ… oraz usĹ‚ugami dla projektu Firma3 â€“ Premium	1	7Â 840,00 zĹ‚	23	1Â 803,20 zĹ‚	7Â 840,00 zĹ‚	9Â 643,20 zĹ‚	126Â 918,13 zĹ‚	156Â 109,30 zĹ‚
-Firma3 sp. z o.o.	ul. Krkusowa 12, 30-123 KrakĂłw	675-152-93-71	2021-01-04	2020-12-30	3-04/01/2021	Firma3 - prace projektowe oraz programistyczne zwiÄ…zane z utrzymaniem i poprawÄ… bĹ‚Ä™dĂłw oraz bieĹĽÄ…cymi dziaĹ‚aniami,  zgodne z zaĹ‚Ä…cznikiem	4	1Â 250,00 zĹ‚	23	1Â 150,00 zĹ‚	5Â 000,00 zĹ‚	6Â 150,00 zĹ‚	126Â 918,13 zĹ‚	156Â 109,30 zĹ‚
-Firma8 Sp. z o.o. sp.k.	ul. Krkusowa 12, 30-123 KrakĂłw	677-00-46-633	2021-01-04	2020-12-30	4-04/01/2021	Firma8 - prace projektowe oraz programistyczne, zgodnie z zaĹ‚Ä…cznikiem	21,01875	1Â 250,00 zĹ‚	23	6Â 042,89 zĹ‚	26Â 273,44 zĹ‚	32Â 316,33 zĹ‚	26Â 273,44 zĹ‚	32Â 316,33 zĹ‚
-Firma9 SP. Z O.O.	ul. Dobra 28, 00-344 Warszawa	118-16-48-603	2021-01-04	2020-12-30	5-04/01/2021	NAJEM SERWERA ZA OKRES 12.2020 (SPECYFIKACJA ZGODNA Z UMOWÄ„)   	1	13Â 000,00 zĹ‚	23	2Â 990,00 zĹ‚	13Â 000,00 zĹ‚	15Â 990,00 zĹ‚	13Â 000,00 zĹ‚	15Â 990,00 zĹ‚
-Firma4	ul. MICKIEWICZA 1/5, 33-100 TARNĂ“W	873-171-75-73	2021-01-12	2020-12-30	1-12/01/2021	Abonament â€“ aktywne karty SIM zgodnie z zaĹ‚Ä…cznikiem 	596,0335	7,50 zĹ‚	23	1Â 028,16	4Â 470,25 zĹ‚	5Â 498,41 zĹ‚	4Â 470,25 zĹ‚	5Â 498,41 zĹ‚
-Firma4	ul. MICKIEWICZA 1/5, 33-100 TARNĂ“W	873-171-75-73	2021-01-12	2020-12-30	2-12/01/2021	UrzÄ…dzenia GPS â€“ terminale/montaĹĽ â€“ listopad 2020 zgodnie z zaĹ‚Ä…cznikiem 	65	280,00 zĹ‚	23	4Â 186,00 zĹ‚	18Â 200,00 zĹ‚	22Â 386,00 zĹ‚	18Â 200,00 zĹ‚	22Â 386,00 zĹ‚
-Firma1 Sp. z o.o	AL. A. Mickiewicza 141, 31-127 KrakĂłw	113-29-95-753 	2021-01-19	2020-12-30	1-19/01/2021	Prace zwiÄ…zane z utrzymaniem aplikacji Aplikacja sprzedaĹĽowa w grudniu 2020, zgodnie z zaĹ‚Ä…cznikiem	8,68750	1Â 000,00 zĹ‚	23	1Â 998,13 zĹ‚	8Â 687,50 zĹ‚	10Â 685,63 zĹ‚	30Â 833,75 zĹ‚	37Â 925,51 zĹ‚
-Firma1 Sp. z o.o	AL. A. Mickiewicza 141, 31-127 KrakĂłw	113-29-95-753 	2021-01-19	2020-12-30	1-19/01/2021	Prace zwiÄ…zane z utrzymaniem aplikacji Sellcar w grudniu 2020, zgodnie z zaĹ‚Ä…cznikiem	10,27750	1Â 000,00 zĹ‚	23	2Â 363,83 zĹ‚	10Â 277,50 zĹ‚	12Â 641,33 zĹ‚	30Â 833,75 zĹ‚	37Â 925,51 zĹ‚
-Firma1 Sp. z o.o	AL. A. Mickiewicza 141, 31-127 KrakĂłw	113-29-95-753 	2021-01-19	2020-12-30	1-19/01/2021	Prace zwiÄ…zane z utrzymaniem systemu Aplikacja GPS w grudniu 2020, zgodnie z zaĹ‚Ä…cznikiem	4,50000	1Â 000,00 zĹ‚	23	1Â 035,00 zĹ‚	4Â 500,00 zĹ‚	5Â 535,00 zĹ‚	30Â 833,75 zĹ‚	37Â 925,51 zĹ‚
-Firma1 Sp. z o.o	AL. A. Mickiewicza 141, 31-127 KrakĂłw	113-29-95-753 	2021-01-19	2020-12-30	1-19/01/2021	Prace zwiÄ…zane z utrzymaniem systemu Aplikacja ubezpieczeniowa w grudniu 2020, zgodnie z zaĹ‚Ä…cznikiem	0,68750	1Â 000,00 zĹ‚	23	158,13 zĹ‚	687,50 zĹ‚	845,63 zĹ‚	30Â 833,75 zĹ‚	37Â 925,51 zĹ‚
-Firma1 Sp. z o.o	AL. A. Mickiewicza 141, 31-127 KrakĂłw	113-29-95-753 	2021-01-19	2020-12-30	1-19/01/2021	Prace zwiÄ…zane z utrzymaniem systemu Aplikacja windykacyjna w grudniu 2020, zgodnie z zaĹ‚Ä…cznikiem	2,31250	1Â 000,00 zĹ‚	23	531,88 zĹ‚	2Â 312,50 zĹ‚	2Â 844,38 zĹ‚	30Â 833,75 zĹ‚	37Â 925,51 zĹ‚
-Firma1 Sp. z o.o	AL. A. Mickiewicza 141, 31-127 KrakĂłw	113-29-95-753 	2021-01-19	2020-12-30	1-19/01/2021	Prace zwiÄ…zane z utrzymaniem systemu Ces w grudniu 2020, zgodnie z zaĹ‚Ä…cznikiem	0,31250	1Â 000,00 zĹ‚	23	71,88 zĹ‚	312,50 zĹ‚	384,38 zĹ‚	30Â 833,75 zĹ‚	37Â 925,51 zĹ‚
-Firma1 Sp. z o.o	AL. A. Mickiewicza 141, 31-127 KrakĂłw	113-29-95-753 	2021-01-19	2020-12-30	1-19/01/2021	Prace zwiÄ…zane z utrzymaniem usĹ‚ugi eFaktura w grudniu 2020, zgodnie z zaĹ‚Ä…cznikiem	0,12500	1Â 000,00 zĹ‚	23	28,75 zĹ‚	125,00 zĹ‚	153,75 zĹ‚	30Â 833,75 zĹ‚	37Â 925,51 zĹ‚
-Firma1 Sp. z o.o	AL. A. Mickiewicza 141, 31-127 KrakĂłw	113-29-95-753 	2021-01-19	2020-12-30	1-19/01/2021	Prace zwiÄ…zane z utrzymaniem systemu Seyo (Portal Klienta) w grudniu 2020, zgodnie z zaĹ‚Ä…cznikiem	0,18750	1Â 000,00 zĹ‚	23	43,13 zĹ‚	187,50 zĹ‚	230,63 zĹ‚	30Â 833,75 zĹ‚	37Â 925,51 zĹ‚
-Firma1 Sp. z o.o	AL. A. Mickiewicza 141, 31-127 KrakĂłw	113-29-95-753 	2021-01-19	2020-12-30	1-19/01/2021	Prace zwiÄ…zane z utrzymaniem â€“ wyceny w grudniu 2020, zgodnie z zaĹ‚Ä…cznikiem	3,74375	1Â 000,00 zĹ‚	23	861,06 zĹ‚	3Â 743,75 zĹ‚	4Â 604,81 zĹ‚	30Â 833,75 zĹ‚	37Â 925,51 zĹ‚
-Firma1 Sp. z o.o	AL. A. Mickiewicza 141, 31-127 KrakĂłw	113-29-95-753 	2021-01-19	2020-12-30	2-19/01/2021	Prace zwiÄ…zane z utrzymaniem infrastruktury w grudniu 2020, zgodnie z zaĹ‚Ä…cznikiem	13,43125	1Â 000,00 zĹ‚	23	3Â 089,19 zĹ‚	13Â 431,25 zĹ‚	16Â 520,44 zĹ‚	13Â 431,25 zĹ‚	16Â 520,44 zĹ‚
-</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="283">
   <si>
     <t>Nazwa odbiorcy</t>
   </si>
@@ -1789,86 +1733,79 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="45.5546875" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" customWidth="1"/>
-    <col min="5" max="5" width="19.88671875" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" customWidth="1"/>
-    <col min="7" max="7" width="23.77734375" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" customWidth="1"/>
-    <col min="9" max="9" width="17" customWidth="1"/>
-    <col min="10" max="10" width="16.77734375" customWidth="1"/>
-    <col min="11" max="11" width="17" customWidth="1"/>
-    <col min="12" max="12" width="17.5546875" customWidth="1"/>
-    <col min="13" max="13" width="22.33203125" customWidth="1"/>
-    <col min="14" max="14" width="24.21875" customWidth="1"/>
-    <col min="15" max="15" width="21.44140625" customWidth="1"/>
-    <col min="16" max="16" width="16.5546875" customWidth="1"/>
+    <col min="1" max="1" width="22.109375" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="15.5546875" customWidth="1"/>
+    <col min="6" max="6" width="14.77734375" customWidth="1"/>
+    <col min="7" max="7" width="14.21875" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>14</v>
-      </c>
-      <c r="O1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>17</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
       </c>
       <c r="D2" s="2">
         <v>44113</v>
@@ -1877,45 +1814,45 @@
         <v>44113</v>
       </c>
       <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
         <v>19</v>
-      </c>
-      <c r="G2" t="s">
-        <v>20</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
       <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2">
+        <v>23</v>
+      </c>
+      <c r="K2" t="s">
         <v>21</v>
       </c>
-      <c r="J2">
-        <v>23</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" t="s">
         <v>22</v>
       </c>
-      <c r="L2" t="s">
-        <v>21</v>
-      </c>
-      <c r="M2" t="s">
-        <v>23</v>
-      </c>
       <c r="N2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
         <v>24</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>25</v>
       </c>
       <c r="D3" s="2">
         <v>44113</v>
@@ -1924,45 +1861,45 @@
         <v>44113</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="I3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3">
+        <v>23</v>
+      </c>
+      <c r="K3" t="s">
         <v>27</v>
       </c>
-      <c r="J3">
-        <v>23</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" t="s">
         <v>28</v>
       </c>
-      <c r="L3" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" t="s">
-        <v>29</v>
-      </c>
       <c r="N3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
         <v>30</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>31</v>
-      </c>
-      <c r="C4" t="s">
-        <v>32</v>
       </c>
       <c r="D4" s="2">
         <v>44117</v>
@@ -1971,45 +1908,45 @@
         <v>44117</v>
       </c>
       <c r="F4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" t="s">
         <v>33</v>
-      </c>
-      <c r="G4" t="s">
-        <v>34</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
       <c r="I4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4">
+        <v>23</v>
+      </c>
+      <c r="K4" t="s">
         <v>35</v>
       </c>
-      <c r="J4">
-        <v>23</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
+        <v>34</v>
+      </c>
+      <c r="M4" t="s">
         <v>36</v>
       </c>
-      <c r="L4" t="s">
-        <v>35</v>
-      </c>
-      <c r="M4" t="s">
-        <v>37</v>
-      </c>
       <c r="N4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="s">
         <v>38</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>39</v>
-      </c>
-      <c r="C5" t="s">
-        <v>40</v>
       </c>
       <c r="D5" s="2">
         <v>44118</v>
@@ -2018,45 +1955,45 @@
         <v>44118</v>
       </c>
       <c r="F5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" t="s">
         <v>41</v>
-      </c>
-      <c r="G5" t="s">
-        <v>42</v>
       </c>
       <c r="H5">
         <v>4.75</v>
       </c>
       <c r="I5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5">
+        <v>23</v>
+      </c>
+      <c r="K5" t="s">
         <v>43</v>
       </c>
-      <c r="J5">
-        <v>23</v>
-      </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>44</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>45</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>46</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>47</v>
-      </c>
-      <c r="O5" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
         <v>38</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>39</v>
-      </c>
-      <c r="C6" t="s">
-        <v>40</v>
       </c>
       <c r="D6" s="2">
         <v>44118</v>
@@ -2065,45 +2002,45 @@
         <v>44118</v>
       </c>
       <c r="F6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H6">
         <v>55</v>
       </c>
       <c r="I6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J6">
         <v>23</v>
       </c>
       <c r="K6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L6" t="s">
         <v>50</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>51</v>
       </c>
-      <c r="M6" t="s">
-        <v>52</v>
-      </c>
       <c r="N6" t="s">
+        <v>46</v>
+      </c>
+      <c r="O6" t="s">
         <v>47</v>
-      </c>
-      <c r="O6" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
         <v>38</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>39</v>
-      </c>
-      <c r="C7" t="s">
-        <v>40</v>
       </c>
       <c r="D7" s="2">
         <v>44118</v>
@@ -2112,45 +2049,45 @@
         <v>44118</v>
       </c>
       <c r="F7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H7">
         <v>10</v>
       </c>
       <c r="I7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J7">
         <v>23</v>
       </c>
       <c r="K7" t="s">
+        <v>53</v>
+      </c>
+      <c r="L7" t="s">
         <v>54</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>55</v>
       </c>
-      <c r="M7" t="s">
-        <v>56</v>
-      </c>
       <c r="N7" t="s">
+        <v>46</v>
+      </c>
+      <c r="O7" t="s">
         <v>47</v>
-      </c>
-      <c r="O7" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
         <v>38</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>39</v>
-      </c>
-      <c r="C8" t="s">
-        <v>40</v>
       </c>
       <c r="D8" s="2">
         <v>44118</v>
@@ -2159,45 +2096,45 @@
         <v>44118</v>
       </c>
       <c r="F8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H8">
         <v>0.75</v>
       </c>
       <c r="I8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J8">
         <v>23</v>
       </c>
       <c r="K8" t="s">
+        <v>57</v>
+      </c>
+      <c r="L8" t="s">
         <v>58</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>59</v>
       </c>
-      <c r="M8" t="s">
-        <v>60</v>
-      </c>
       <c r="N8" t="s">
+        <v>46</v>
+      </c>
+      <c r="O8" t="s">
         <v>47</v>
-      </c>
-      <c r="O8" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
         <v>38</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>39</v>
-      </c>
-      <c r="C9" t="s">
-        <v>40</v>
       </c>
       <c r="D9" s="2">
         <v>44118</v>
@@ -2206,45 +2143,45 @@
         <v>44118</v>
       </c>
       <c r="F9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H9">
         <v>2</v>
       </c>
       <c r="I9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J9">
         <v>23</v>
       </c>
       <c r="K9" t="s">
+        <v>61</v>
+      </c>
+      <c r="L9" t="s">
         <v>62</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>63</v>
       </c>
-      <c r="M9" t="s">
-        <v>64</v>
-      </c>
       <c r="N9" t="s">
+        <v>46</v>
+      </c>
+      <c r="O9" t="s">
         <v>47</v>
-      </c>
-      <c r="O9" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
         <v>38</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>39</v>
-      </c>
-      <c r="C10" t="s">
-        <v>40</v>
       </c>
       <c r="D10" s="2">
         <v>44118</v>
@@ -2253,45 +2190,45 @@
         <v>44118</v>
       </c>
       <c r="F10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H10">
         <v>1.5</v>
       </c>
       <c r="I10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J10">
         <v>23</v>
       </c>
       <c r="K10" t="s">
+        <v>65</v>
+      </c>
+      <c r="L10" t="s">
         <v>66</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>67</v>
       </c>
-      <c r="M10" t="s">
-        <v>68</v>
-      </c>
       <c r="N10" t="s">
+        <v>46</v>
+      </c>
+      <c r="O10" t="s">
         <v>47</v>
-      </c>
-      <c r="O10" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" t="s">
         <v>38</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>39</v>
-      </c>
-      <c r="C11" t="s">
-        <v>40</v>
       </c>
       <c r="D11" s="2">
         <v>44118</v>
@@ -2300,45 +2237,45 @@
         <v>44118</v>
       </c>
       <c r="F11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H11">
         <v>2.25</v>
       </c>
       <c r="I11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J11">
         <v>23</v>
       </c>
       <c r="K11" t="s">
+        <v>69</v>
+      </c>
+      <c r="L11" t="s">
         <v>70</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>71</v>
       </c>
-      <c r="M11" t="s">
-        <v>72</v>
-      </c>
       <c r="N11" t="s">
+        <v>46</v>
+      </c>
+      <c r="O11" t="s">
         <v>47</v>
-      </c>
-      <c r="O11" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" t="s">
         <v>73</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>74</v>
-      </c>
-      <c r="C12" t="s">
-        <v>75</v>
       </c>
       <c r="D12" s="2">
         <v>44119</v>
@@ -2347,45 +2284,45 @@
         <v>44119</v>
       </c>
       <c r="F12" t="s">
+        <v>75</v>
+      </c>
+      <c r="G12" t="s">
         <v>76</v>
-      </c>
-      <c r="G12" t="s">
-        <v>77</v>
       </c>
       <c r="H12">
         <v>1</v>
       </c>
       <c r="I12" t="s">
+        <v>77</v>
+      </c>
+      <c r="J12">
+        <v>23</v>
+      </c>
+      <c r="K12" t="s">
         <v>78</v>
       </c>
-      <c r="J12">
-        <v>23</v>
-      </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
+        <v>77</v>
+      </c>
+      <c r="M12" t="s">
         <v>79</v>
       </c>
-      <c r="L12" t="s">
-        <v>78</v>
-      </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>80</v>
       </c>
-      <c r="N12" t="s">
+      <c r="O12" t="s">
         <v>81</v>
-      </c>
-      <c r="O12" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" t="s">
         <v>73</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>74</v>
-      </c>
-      <c r="C13" t="s">
-        <v>75</v>
       </c>
       <c r="D13" s="2">
         <v>44119</v>
@@ -2394,45 +2331,45 @@
         <v>44119</v>
       </c>
       <c r="F13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H13">
         <v>1</v>
       </c>
       <c r="I13" t="s">
+        <v>83</v>
+      </c>
+      <c r="J13">
+        <v>23</v>
+      </c>
+      <c r="K13" t="s">
         <v>84</v>
       </c>
-      <c r="J13">
-        <v>23</v>
-      </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
+        <v>83</v>
+      </c>
+      <c r="M13" t="s">
         <v>85</v>
       </c>
-      <c r="L13" t="s">
-        <v>84</v>
-      </c>
-      <c r="M13" t="s">
-        <v>86</v>
-      </c>
       <c r="N13" t="s">
+        <v>80</v>
+      </c>
+      <c r="O13" t="s">
         <v>81</v>
-      </c>
-      <c r="O13" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" t="s">
         <v>73</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>74</v>
-      </c>
-      <c r="C14" t="s">
-        <v>75</v>
       </c>
       <c r="D14" s="2">
         <v>44119</v>
@@ -2441,45 +2378,45 @@
         <v>44119</v>
       </c>
       <c r="F14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H14">
         <v>1</v>
       </c>
       <c r="I14" t="s">
+        <v>87</v>
+      </c>
+      <c r="J14">
+        <v>23</v>
+      </c>
+      <c r="K14" t="s">
         <v>88</v>
       </c>
-      <c r="J14">
-        <v>23</v>
-      </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
+        <v>87</v>
+      </c>
+      <c r="M14" t="s">
         <v>89</v>
       </c>
-      <c r="L14" t="s">
-        <v>88</v>
-      </c>
-      <c r="M14" t="s">
-        <v>90</v>
-      </c>
       <c r="N14" t="s">
+        <v>80</v>
+      </c>
+      <c r="O14" t="s">
         <v>81</v>
-      </c>
-      <c r="O14" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" t="s">
         <v>73</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>74</v>
-      </c>
-      <c r="C15" t="s">
-        <v>75</v>
       </c>
       <c r="D15" s="2">
         <v>44119</v>
@@ -2488,45 +2425,45 @@
         <v>44119</v>
       </c>
       <c r="F15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H15">
         <v>1</v>
       </c>
       <c r="I15" t="s">
+        <v>91</v>
+      </c>
+      <c r="J15">
+        <v>23</v>
+      </c>
+      <c r="K15" t="s">
         <v>92</v>
       </c>
-      <c r="J15">
-        <v>23</v>
-      </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
+        <v>91</v>
+      </c>
+      <c r="M15" t="s">
         <v>93</v>
       </c>
-      <c r="L15" t="s">
-        <v>92</v>
-      </c>
-      <c r="M15" t="s">
-        <v>94</v>
-      </c>
       <c r="N15" t="s">
+        <v>80</v>
+      </c>
+      <c r="O15" t="s">
         <v>81</v>
-      </c>
-      <c r="O15" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" t="s">
         <v>73</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>74</v>
-      </c>
-      <c r="C16" t="s">
-        <v>75</v>
       </c>
       <c r="D16" s="2">
         <v>44119</v>
@@ -2535,45 +2472,45 @@
         <v>44119</v>
       </c>
       <c r="F16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H16">
         <v>1</v>
       </c>
       <c r="I16" t="s">
+        <v>95</v>
+      </c>
+      <c r="J16">
+        <v>23</v>
+      </c>
+      <c r="K16" t="s">
         <v>96</v>
       </c>
-      <c r="J16">
-        <v>23</v>
-      </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
+        <v>95</v>
+      </c>
+      <c r="M16" t="s">
         <v>97</v>
       </c>
-      <c r="L16" t="s">
-        <v>96</v>
-      </c>
-      <c r="M16" t="s">
-        <v>98</v>
-      </c>
       <c r="N16" t="s">
+        <v>80</v>
+      </c>
+      <c r="O16" t="s">
         <v>81</v>
-      </c>
-      <c r="O16" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" t="s">
         <v>73</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>74</v>
-      </c>
-      <c r="C17" t="s">
-        <v>75</v>
       </c>
       <c r="D17" s="2">
         <v>44119</v>
@@ -2582,45 +2519,45 @@
         <v>44119</v>
       </c>
       <c r="F17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H17">
         <v>1</v>
       </c>
       <c r="I17" t="s">
+        <v>99</v>
+      </c>
+      <c r="J17">
+        <v>23</v>
+      </c>
+      <c r="K17" t="s">
         <v>100</v>
       </c>
-      <c r="J17">
-        <v>23</v>
-      </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
+        <v>99</v>
+      </c>
+      <c r="M17" t="s">
         <v>101</v>
       </c>
-      <c r="L17" t="s">
-        <v>100</v>
-      </c>
-      <c r="M17" t="s">
-        <v>102</v>
-      </c>
       <c r="N17" t="s">
+        <v>80</v>
+      </c>
+      <c r="O17" t="s">
         <v>81</v>
-      </c>
-      <c r="O17" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" t="s">
         <v>73</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>74</v>
-      </c>
-      <c r="C18" t="s">
-        <v>75</v>
       </c>
       <c r="D18" s="2">
         <v>44119</v>
@@ -2629,45 +2566,45 @@
         <v>44119</v>
       </c>
       <c r="F18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H18">
         <v>1</v>
       </c>
       <c r="I18" t="s">
+        <v>103</v>
+      </c>
+      <c r="J18">
+        <v>23</v>
+      </c>
+      <c r="K18" t="s">
         <v>104</v>
       </c>
-      <c r="J18">
-        <v>23</v>
-      </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
+        <v>103</v>
+      </c>
+      <c r="M18" t="s">
         <v>105</v>
       </c>
-      <c r="L18" t="s">
-        <v>104</v>
-      </c>
-      <c r="M18" t="s">
-        <v>106</v>
-      </c>
       <c r="N18" t="s">
+        <v>80</v>
+      </c>
+      <c r="O18" t="s">
         <v>81</v>
-      </c>
-      <c r="O18" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" t="s">
         <v>73</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>74</v>
-      </c>
-      <c r="C19" t="s">
-        <v>75</v>
       </c>
       <c r="D19" s="2">
         <v>44119</v>
@@ -2676,45 +2613,45 @@
         <v>44119</v>
       </c>
       <c r="F19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G19" t="s">
         <v>107</v>
-      </c>
-      <c r="G19" t="s">
-        <v>108</v>
       </c>
       <c r="H19">
         <v>1</v>
       </c>
       <c r="I19" t="s">
+        <v>108</v>
+      </c>
+      <c r="J19">
+        <v>23</v>
+      </c>
+      <c r="K19" t="s">
         <v>109</v>
       </c>
-      <c r="J19">
-        <v>23</v>
-      </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
+        <v>108</v>
+      </c>
+      <c r="M19" t="s">
         <v>110</v>
       </c>
-      <c r="L19" t="s">
-        <v>109</v>
-      </c>
-      <c r="M19" t="s">
+      <c r="N19" t="s">
         <v>111</v>
       </c>
-      <c r="N19" t="s">
+      <c r="O19" t="s">
         <v>112</v>
-      </c>
-      <c r="O19" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" t="s">
         <v>73</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>74</v>
-      </c>
-      <c r="C20" t="s">
-        <v>75</v>
       </c>
       <c r="D20" s="2">
         <v>44119</v>
@@ -2723,45 +2660,45 @@
         <v>44119</v>
       </c>
       <c r="F20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H20">
         <v>1</v>
       </c>
       <c r="I20" t="s">
+        <v>54</v>
+      </c>
+      <c r="J20">
+        <v>23</v>
+      </c>
+      <c r="K20" t="s">
+        <v>53</v>
+      </c>
+      <c r="L20" t="s">
+        <v>54</v>
+      </c>
+      <c r="M20" t="s">
         <v>55</v>
       </c>
-      <c r="J20">
-        <v>23</v>
-      </c>
-      <c r="K20" t="s">
-        <v>54</v>
-      </c>
-      <c r="L20" t="s">
-        <v>55</v>
-      </c>
-      <c r="M20" t="s">
-        <v>56</v>
-      </c>
       <c r="N20" t="s">
+        <v>111</v>
+      </c>
+      <c r="O20" t="s">
         <v>112</v>
-      </c>
-      <c r="O20" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" t="s">
         <v>73</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>74</v>
-      </c>
-      <c r="C21" t="s">
-        <v>75</v>
       </c>
       <c r="D21" s="2">
         <v>44119</v>
@@ -2770,45 +2707,45 @@
         <v>44119</v>
       </c>
       <c r="F21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H21">
         <v>1</v>
       </c>
       <c r="I21" t="s">
+        <v>115</v>
+      </c>
+      <c r="J21">
+        <v>23</v>
+      </c>
+      <c r="K21" t="s">
         <v>116</v>
       </c>
-      <c r="J21">
-        <v>23</v>
-      </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
+        <v>115</v>
+      </c>
+      <c r="M21" t="s">
         <v>117</v>
       </c>
-      <c r="L21" t="s">
-        <v>116</v>
-      </c>
-      <c r="M21" t="s">
-        <v>118</v>
-      </c>
       <c r="N21" t="s">
+        <v>111</v>
+      </c>
+      <c r="O21" t="s">
         <v>112</v>
-      </c>
-      <c r="O21" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22" t="s">
         <v>73</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>74</v>
-      </c>
-      <c r="C22" t="s">
-        <v>75</v>
       </c>
       <c r="D22" s="2">
         <v>44119</v>
@@ -2817,45 +2754,45 @@
         <v>44119</v>
       </c>
       <c r="F22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H22">
         <v>1</v>
       </c>
       <c r="I22" t="s">
+        <v>119</v>
+      </c>
+      <c r="J22">
+        <v>23</v>
+      </c>
+      <c r="K22" t="s">
         <v>120</v>
       </c>
-      <c r="J22">
-        <v>23</v>
-      </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
+        <v>119</v>
+      </c>
+      <c r="M22" t="s">
         <v>121</v>
       </c>
-      <c r="L22" t="s">
-        <v>120</v>
-      </c>
-      <c r="M22" t="s">
-        <v>122</v>
-      </c>
       <c r="N22" t="s">
+        <v>111</v>
+      </c>
+      <c r="O22" t="s">
         <v>112</v>
-      </c>
-      <c r="O22" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" t="s">
         <v>73</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>74</v>
-      </c>
-      <c r="C23" t="s">
-        <v>75</v>
       </c>
       <c r="D23" s="2">
         <v>44119</v>
@@ -2864,45 +2801,45 @@
         <v>44119</v>
       </c>
       <c r="F23" t="s">
+        <v>122</v>
+      </c>
+      <c r="G23" t="s">
         <v>123</v>
-      </c>
-      <c r="G23" t="s">
-        <v>124</v>
       </c>
       <c r="H23">
         <v>24</v>
       </c>
       <c r="I23" t="s">
+        <v>124</v>
+      </c>
+      <c r="J23">
+        <v>23</v>
+      </c>
+      <c r="K23" t="s">
         <v>125</v>
       </c>
-      <c r="J23">
-        <v>23</v>
-      </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>126</v>
       </c>
-      <c r="L23" t="s">
+      <c r="M23" t="s">
         <v>127</v>
       </c>
-      <c r="M23" t="s">
+      <c r="N23" t="s">
         <v>128</v>
       </c>
-      <c r="N23" t="s">
+      <c r="O23" t="s">
         <v>129</v>
-      </c>
-      <c r="O23" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" t="s">
         <v>73</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>74</v>
-      </c>
-      <c r="C24" t="s">
-        <v>75</v>
       </c>
       <c r="D24" s="2">
         <v>44119</v>
@@ -2911,45 +2848,45 @@
         <v>44119</v>
       </c>
       <c r="F24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H24">
         <v>24</v>
       </c>
       <c r="I24" t="s">
+        <v>131</v>
+      </c>
+      <c r="J24">
+        <v>23</v>
+      </c>
+      <c r="K24" t="s">
         <v>132</v>
       </c>
-      <c r="J24">
-        <v>23</v>
-      </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
         <v>133</v>
       </c>
-      <c r="L24" t="s">
+      <c r="M24" t="s">
         <v>134</v>
       </c>
-      <c r="M24" t="s">
-        <v>135</v>
-      </c>
       <c r="N24" t="s">
+        <v>128</v>
+      </c>
+      <c r="O24" t="s">
         <v>129</v>
-      </c>
-      <c r="O24" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" t="s">
         <v>73</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>74</v>
-      </c>
-      <c r="C25" t="s">
-        <v>75</v>
       </c>
       <c r="D25" s="2">
         <v>44119</v>
@@ -2958,45 +2895,45 @@
         <v>44119</v>
       </c>
       <c r="F25" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H25">
         <v>24</v>
       </c>
       <c r="I25" t="s">
+        <v>131</v>
+      </c>
+      <c r="J25">
+        <v>23</v>
+      </c>
+      <c r="K25" t="s">
         <v>132</v>
       </c>
-      <c r="J25">
-        <v>23</v>
-      </c>
-      <c r="K25" t="s">
+      <c r="L25" t="s">
         <v>133</v>
       </c>
-      <c r="L25" t="s">
+      <c r="M25" t="s">
         <v>134</v>
       </c>
-      <c r="M25" t="s">
-        <v>135</v>
-      </c>
       <c r="N25" t="s">
+        <v>128</v>
+      </c>
+      <c r="O25" t="s">
         <v>129</v>
-      </c>
-      <c r="O25" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" t="s">
         <v>73</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>74</v>
-      </c>
-      <c r="C26" t="s">
-        <v>75</v>
       </c>
       <c r="D26" s="2">
         <v>44119</v>
@@ -3005,45 +2942,45 @@
         <v>44119</v>
       </c>
       <c r="F26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H26">
         <v>2</v>
       </c>
       <c r="I26" t="s">
+        <v>137</v>
+      </c>
+      <c r="J26">
+        <v>23</v>
+      </c>
+      <c r="K26" t="s">
         <v>138</v>
       </c>
-      <c r="J26">
-        <v>23</v>
-      </c>
-      <c r="K26" t="s">
+      <c r="L26" t="s">
         <v>139</v>
       </c>
-      <c r="L26" t="s">
-        <v>140</v>
-      </c>
       <c r="M26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N26" t="s">
+        <v>128</v>
+      </c>
+      <c r="O26" t="s">
         <v>129</v>
-      </c>
-      <c r="O26" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" t="s">
         <v>73</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>74</v>
-      </c>
-      <c r="C27" t="s">
-        <v>75</v>
       </c>
       <c r="D27" s="2">
         <v>44119</v>
@@ -3052,45 +2989,45 @@
         <v>44119</v>
       </c>
       <c r="F27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H27">
         <v>2</v>
       </c>
       <c r="I27" t="s">
+        <v>141</v>
+      </c>
+      <c r="J27">
+        <v>23</v>
+      </c>
+      <c r="K27" t="s">
         <v>142</v>
       </c>
-      <c r="J27">
-        <v>23</v>
-      </c>
-      <c r="K27" t="s">
+      <c r="L27" t="s">
         <v>143</v>
       </c>
-      <c r="L27" t="s">
+      <c r="M27" t="s">
         <v>144</v>
       </c>
-      <c r="M27" t="s">
-        <v>145</v>
-      </c>
       <c r="N27" t="s">
+        <v>128</v>
+      </c>
+      <c r="O27" t="s">
         <v>129</v>
-      </c>
-      <c r="O27" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" t="s">
         <v>73</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>74</v>
-      </c>
-      <c r="C28" t="s">
-        <v>75</v>
       </c>
       <c r="D28" s="2">
         <v>44119</v>
@@ -3099,45 +3036,45 @@
         <v>44119</v>
       </c>
       <c r="F28" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G28" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H28">
         <v>28</v>
       </c>
       <c r="I28" t="s">
+        <v>146</v>
+      </c>
+      <c r="J28">
+        <v>23</v>
+      </c>
+      <c r="K28" t="s">
         <v>147</v>
       </c>
-      <c r="J28">
-        <v>23</v>
-      </c>
-      <c r="K28" t="s">
+      <c r="L28" t="s">
         <v>148</v>
       </c>
-      <c r="L28" t="s">
+      <c r="M28" t="s">
         <v>149</v>
       </c>
-      <c r="M28" t="s">
-        <v>150</v>
-      </c>
       <c r="N28" t="s">
+        <v>128</v>
+      </c>
+      <c r="O28" t="s">
         <v>129</v>
-      </c>
-      <c r="O28" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" t="s">
         <v>73</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>74</v>
-      </c>
-      <c r="C29" t="s">
-        <v>75</v>
       </c>
       <c r="D29" s="2">
         <v>44119</v>
@@ -3146,45 +3083,45 @@
         <v>44119</v>
       </c>
       <c r="F29" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G29" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H29">
         <v>24</v>
       </c>
       <c r="I29" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J29">
         <v>23</v>
       </c>
       <c r="K29" t="s">
+        <v>147</v>
+      </c>
+      <c r="L29" t="s">
         <v>148</v>
       </c>
-      <c r="L29" t="s">
+      <c r="M29" t="s">
         <v>149</v>
       </c>
-      <c r="M29" t="s">
-        <v>150</v>
-      </c>
       <c r="N29" t="s">
+        <v>128</v>
+      </c>
+      <c r="O29" t="s">
         <v>129</v>
-      </c>
-      <c r="O29" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" t="s">
         <v>73</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>74</v>
-      </c>
-      <c r="C30" t="s">
-        <v>75</v>
       </c>
       <c r="D30" s="2">
         <v>44120</v>
@@ -3193,45 +3130,45 @@
         <v>44120</v>
       </c>
       <c r="F30" t="s">
+        <v>152</v>
+      </c>
+      <c r="G30" t="s">
         <v>153</v>
-      </c>
-      <c r="G30" t="s">
-        <v>154</v>
       </c>
       <c r="H30">
         <v>1</v>
       </c>
       <c r="I30" t="s">
+        <v>154</v>
+      </c>
+      <c r="J30">
+        <v>23</v>
+      </c>
+      <c r="K30" t="s">
         <v>155</v>
       </c>
-      <c r="J30">
-        <v>23</v>
-      </c>
-      <c r="K30" t="s">
+      <c r="L30" t="s">
+        <v>154</v>
+      </c>
+      <c r="M30" t="s">
         <v>156</v>
       </c>
-      <c r="L30" t="s">
-        <v>155</v>
-      </c>
-      <c r="M30" t="s">
-        <v>157</v>
-      </c>
       <c r="N30" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="O30" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>157</v>
+      </c>
+      <c r="B31" t="s">
         <v>158</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>159</v>
-      </c>
-      <c r="C31" t="s">
-        <v>160</v>
       </c>
       <c r="D31" s="2">
         <v>44140</v>
@@ -3240,45 +3177,45 @@
         <v>44134</v>
       </c>
       <c r="F31" t="s">
+        <v>160</v>
+      </c>
+      <c r="G31" t="s">
         <v>161</v>
-      </c>
-      <c r="G31" t="s">
-        <v>162</v>
       </c>
       <c r="H31">
         <v>1</v>
       </c>
       <c r="I31" t="s">
+        <v>162</v>
+      </c>
+      <c r="J31">
+        <v>23</v>
+      </c>
+      <c r="K31" t="s">
         <v>163</v>
       </c>
-      <c r="J31">
-        <v>23</v>
-      </c>
-      <c r="K31" t="s">
+      <c r="L31" t="s">
+        <v>162</v>
+      </c>
+      <c r="M31" t="s">
         <v>164</v>
       </c>
-      <c r="L31" t="s">
-        <v>163</v>
-      </c>
-      <c r="M31" t="s">
-        <v>165</v>
-      </c>
       <c r="N31" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O31" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>165</v>
+      </c>
+      <c r="B32" t="s">
         <v>166</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>167</v>
-      </c>
-      <c r="C32" t="s">
-        <v>168</v>
       </c>
       <c r="D32" s="2">
         <v>44140</v>
@@ -3287,45 +3224,45 @@
         <v>44134</v>
       </c>
       <c r="F32" t="s">
+        <v>168</v>
+      </c>
+      <c r="G32" t="s">
         <v>169</v>
-      </c>
-      <c r="G32" t="s">
-        <v>170</v>
       </c>
       <c r="H32">
         <v>1</v>
       </c>
       <c r="I32" t="s">
+        <v>170</v>
+      </c>
+      <c r="J32">
+        <v>23</v>
+      </c>
+      <c r="K32" t="s">
         <v>171</v>
       </c>
-      <c r="J32">
-        <v>23</v>
-      </c>
-      <c r="K32" t="s">
+      <c r="L32" t="s">
+        <v>170</v>
+      </c>
+      <c r="M32" t="s">
         <v>172</v>
       </c>
-      <c r="L32" t="s">
-        <v>171</v>
-      </c>
-      <c r="M32" t="s">
-        <v>173</v>
-      </c>
       <c r="N32" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="O32" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>173</v>
+      </c>
+      <c r="B33" t="s">
         <v>174</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>175</v>
-      </c>
-      <c r="C33" t="s">
-        <v>176</v>
       </c>
       <c r="D33" s="2">
         <v>44140</v>
@@ -3334,45 +3271,45 @@
         <v>44134</v>
       </c>
       <c r="F33" t="s">
+        <v>176</v>
+      </c>
+      <c r="G33" t="s">
         <v>177</v>
-      </c>
-      <c r="G33" t="s">
-        <v>178</v>
       </c>
       <c r="H33">
         <v>63</v>
       </c>
       <c r="I33" t="s">
+        <v>178</v>
+      </c>
+      <c r="J33">
+        <v>23</v>
+      </c>
+      <c r="K33" t="s">
         <v>179</v>
       </c>
-      <c r="J33">
-        <v>23</v>
-      </c>
-      <c r="K33" t="s">
+      <c r="L33" t="s">
         <v>180</v>
       </c>
-      <c r="L33" t="s">
+      <c r="M33" t="s">
         <v>181</v>
       </c>
-      <c r="M33" t="s">
-        <v>182</v>
-      </c>
       <c r="N33" t="s">
+        <v>180</v>
+      </c>
+      <c r="O33" t="s">
         <v>181</v>
-      </c>
-      <c r="O33" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>165</v>
+      </c>
+      <c r="B34" t="s">
         <v>166</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>167</v>
-      </c>
-      <c r="C34" t="s">
-        <v>168</v>
       </c>
       <c r="D34" s="2">
         <v>44144</v>
@@ -3381,45 +3318,45 @@
         <v>44134</v>
       </c>
       <c r="F34" t="s">
+        <v>182</v>
+      </c>
+      <c r="G34" t="s">
         <v>183</v>
-      </c>
-      <c r="G34" t="s">
-        <v>184</v>
       </c>
       <c r="H34">
         <v>83.637500000000003</v>
       </c>
       <c r="I34" t="s">
+        <v>184</v>
+      </c>
+      <c r="J34">
+        <v>23</v>
+      </c>
+      <c r="K34" t="s">
         <v>185</v>
       </c>
-      <c r="J34">
-        <v>23</v>
-      </c>
-      <c r="K34" t="s">
+      <c r="L34" t="s">
         <v>186</v>
       </c>
-      <c r="L34" t="s">
+      <c r="M34" t="s">
         <v>187</v>
       </c>
-      <c r="M34" t="s">
+      <c r="N34" t="s">
         <v>188</v>
       </c>
-      <c r="N34" t="s">
+      <c r="O34" t="s">
         <v>189</v>
-      </c>
-      <c r="O34" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>165</v>
+      </c>
+      <c r="B35" t="s">
         <v>166</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>167</v>
-      </c>
-      <c r="C35" t="s">
-        <v>168</v>
       </c>
       <c r="D35" s="2">
         <v>44144</v>
@@ -3428,45 +3365,45 @@
         <v>44134</v>
       </c>
       <c r="F35" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G35" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H35">
         <v>1</v>
       </c>
       <c r="I35" t="s">
+        <v>191</v>
+      </c>
+      <c r="J35">
+        <v>23</v>
+      </c>
+      <c r="K35" t="s">
         <v>192</v>
       </c>
-      <c r="J35">
-        <v>23</v>
-      </c>
-      <c r="K35" t="s">
+      <c r="L35" t="s">
+        <v>191</v>
+      </c>
+      <c r="M35" t="s">
         <v>193</v>
       </c>
-      <c r="L35" t="s">
-        <v>192</v>
-      </c>
-      <c r="M35" t="s">
-        <v>194</v>
-      </c>
       <c r="N35" t="s">
+        <v>188</v>
+      </c>
+      <c r="O35" t="s">
         <v>189</v>
-      </c>
-      <c r="O35" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>165</v>
+      </c>
+      <c r="B36" t="s">
         <v>166</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>167</v>
-      </c>
-      <c r="C36" t="s">
-        <v>168</v>
       </c>
       <c r="D36" s="2">
         <v>44144</v>
@@ -3475,45 +3412,45 @@
         <v>44134</v>
       </c>
       <c r="F36" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H36">
         <v>4</v>
       </c>
       <c r="I36" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J36">
         <v>23</v>
       </c>
       <c r="K36" t="s">
+        <v>120</v>
+      </c>
+      <c r="L36" t="s">
+        <v>119</v>
+      </c>
+      <c r="M36" t="s">
         <v>121</v>
       </c>
-      <c r="L36" t="s">
-        <v>120</v>
-      </c>
-      <c r="M36" t="s">
-        <v>122</v>
-      </c>
       <c r="N36" t="s">
+        <v>188</v>
+      </c>
+      <c r="O36" t="s">
         <v>189</v>
-      </c>
-      <c r="O36" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>165</v>
+      </c>
+      <c r="B37" t="s">
         <v>166</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>167</v>
-      </c>
-      <c r="C37" t="s">
-        <v>168</v>
       </c>
       <c r="D37" s="2">
         <v>44144</v>
@@ -3522,45 +3459,45 @@
         <v>44134</v>
       </c>
       <c r="F37" t="s">
+        <v>195</v>
+      </c>
+      <c r="G37" t="s">
         <v>196</v>
-      </c>
-      <c r="G37" t="s">
-        <v>197</v>
       </c>
       <c r="H37">
         <v>12.1875</v>
       </c>
       <c r="I37" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J37">
         <v>23</v>
       </c>
       <c r="K37" t="s">
+        <v>197</v>
+      </c>
+      <c r="L37" t="s">
         <v>198</v>
       </c>
-      <c r="L37" t="s">
+      <c r="M37" t="s">
         <v>199</v>
       </c>
-      <c r="M37" t="s">
+      <c r="N37" t="s">
         <v>200</v>
       </c>
-      <c r="N37" t="s">
+      <c r="O37" t="s">
         <v>201</v>
-      </c>
-      <c r="O37" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>165</v>
+      </c>
+      <c r="B38" t="s">
         <v>166</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>167</v>
-      </c>
-      <c r="C38" t="s">
-        <v>168</v>
       </c>
       <c r="D38" s="2">
         <v>44144</v>
@@ -3569,45 +3506,45 @@
         <v>44134</v>
       </c>
       <c r="F38" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G38" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H38">
         <v>6.5</v>
       </c>
       <c r="I38" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J38">
         <v>23</v>
       </c>
       <c r="K38" t="s">
+        <v>203</v>
+      </c>
+      <c r="L38" t="s">
         <v>204</v>
       </c>
-      <c r="L38" t="s">
+      <c r="M38" t="s">
         <v>205</v>
       </c>
-      <c r="M38" t="s">
-        <v>206</v>
-      </c>
       <c r="N38" t="s">
+        <v>200</v>
+      </c>
+      <c r="O38" t="s">
         <v>201</v>
-      </c>
-      <c r="O38" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>165</v>
+      </c>
+      <c r="B39" t="s">
         <v>166</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>167</v>
-      </c>
-      <c r="C39" t="s">
-        <v>168</v>
       </c>
       <c r="D39" s="2">
         <v>44147</v>
@@ -3616,45 +3553,45 @@
         <v>44147</v>
       </c>
       <c r="F39" t="s">
+        <v>206</v>
+      </c>
+      <c r="G39" t="s">
         <v>207</v>
-      </c>
-      <c r="G39" t="s">
-        <v>208</v>
       </c>
       <c r="H39">
         <v>-0.8125</v>
       </c>
       <c r="I39" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J39">
         <v>23</v>
       </c>
       <c r="K39" t="s">
+        <v>208</v>
+      </c>
+      <c r="L39" t="s">
         <v>209</v>
       </c>
-      <c r="L39" t="s">
+      <c r="M39" t="s">
         <v>210</v>
       </c>
-      <c r="M39" t="s">
-        <v>211</v>
-      </c>
       <c r="N39" t="s">
+        <v>209</v>
+      </c>
+      <c r="O39" t="s">
         <v>210</v>
-      </c>
-      <c r="O39" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>211</v>
+      </c>
+      <c r="B40" t="s">
+        <v>166</v>
+      </c>
+      <c r="C40" t="s">
         <v>212</v>
-      </c>
-      <c r="B40" t="s">
-        <v>167</v>
-      </c>
-      <c r="C40" t="s">
-        <v>213</v>
       </c>
       <c r="D40" s="2">
         <v>44145</v>
@@ -3663,45 +3600,45 @@
         <v>44134</v>
       </c>
       <c r="F40" t="s">
+        <v>213</v>
+      </c>
+      <c r="G40" t="s">
         <v>214</v>
-      </c>
-      <c r="G40" t="s">
-        <v>215</v>
       </c>
       <c r="H40">
         <v>26.475000000000001</v>
       </c>
       <c r="I40" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J40">
         <v>23</v>
       </c>
       <c r="K40" t="s">
+        <v>215</v>
+      </c>
+      <c r="L40" t="s">
         <v>216</v>
       </c>
-      <c r="L40" t="s">
+      <c r="M40" t="s">
         <v>217</v>
       </c>
-      <c r="M40" t="s">
-        <v>218</v>
-      </c>
       <c r="N40" t="s">
+        <v>216</v>
+      </c>
+      <c r="O40" t="s">
         <v>217</v>
-      </c>
-      <c r="O40" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>15</v>
+      </c>
+      <c r="B41" t="s">
         <v>16</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>17</v>
-      </c>
-      <c r="C41" t="s">
-        <v>18</v>
       </c>
       <c r="D41" s="2">
         <v>44145</v>
@@ -3710,45 +3647,45 @@
         <v>44145</v>
       </c>
       <c r="F41" t="s">
+        <v>218</v>
+      </c>
+      <c r="G41" t="s">
         <v>219</v>
-      </c>
-      <c r="G41" t="s">
-        <v>220</v>
       </c>
       <c r="H41">
         <v>1</v>
       </c>
       <c r="I41" t="s">
+        <v>20</v>
+      </c>
+      <c r="J41">
+        <v>23</v>
+      </c>
+      <c r="K41" t="s">
         <v>21</v>
       </c>
-      <c r="J41">
-        <v>23</v>
-      </c>
-      <c r="K41" t="s">
+      <c r="L41" t="s">
+        <v>20</v>
+      </c>
+      <c r="M41" t="s">
         <v>22</v>
       </c>
-      <c r="L41" t="s">
-        <v>21</v>
-      </c>
-      <c r="M41" t="s">
-        <v>23</v>
-      </c>
       <c r="N41" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O41" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>23</v>
+      </c>
+      <c r="B42" t="s">
+        <v>16</v>
+      </c>
+      <c r="C42" t="s">
         <v>24</v>
-      </c>
-      <c r="B42" t="s">
-        <v>17</v>
-      </c>
-      <c r="C42" t="s">
-        <v>25</v>
       </c>
       <c r="D42" s="2">
         <v>44145</v>
@@ -3757,45 +3694,45 @@
         <v>44145</v>
       </c>
       <c r="F42" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G42" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H42">
         <v>1</v>
       </c>
       <c r="I42" t="s">
+        <v>26</v>
+      </c>
+      <c r="J42">
+        <v>23</v>
+      </c>
+      <c r="K42" t="s">
         <v>27</v>
       </c>
-      <c r="J42">
-        <v>23</v>
-      </c>
-      <c r="K42" t="s">
+      <c r="L42" t="s">
+        <v>26</v>
+      </c>
+      <c r="M42" t="s">
         <v>28</v>
       </c>
-      <c r="L42" t="s">
-        <v>27</v>
-      </c>
-      <c r="M42" t="s">
-        <v>29</v>
-      </c>
       <c r="N42" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O42" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
+        <v>173</v>
+      </c>
+      <c r="B43" t="s">
         <v>174</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
         <v>175</v>
-      </c>
-      <c r="C43" t="s">
-        <v>176</v>
       </c>
       <c r="D43" s="2">
         <v>44148</v>
@@ -3804,45 +3741,45 @@
         <v>44134</v>
       </c>
       <c r="F43" t="s">
+        <v>221</v>
+      </c>
+      <c r="G43" t="s">
         <v>222</v>
-      </c>
-      <c r="G43" t="s">
-        <v>223</v>
       </c>
       <c r="H43">
         <v>472.93369999999999</v>
       </c>
       <c r="I43" t="s">
+        <v>223</v>
+      </c>
+      <c r="J43">
+        <v>23</v>
+      </c>
+      <c r="K43" t="s">
         <v>224</v>
       </c>
-      <c r="J43">
-        <v>23</v>
-      </c>
-      <c r="K43" t="s">
+      <c r="L43" t="s">
         <v>225</v>
       </c>
-      <c r="L43" t="s">
+      <c r="M43" t="s">
         <v>226</v>
       </c>
-      <c r="M43" t="s">
-        <v>227</v>
-      </c>
       <c r="N43" t="s">
+        <v>225</v>
+      </c>
+      <c r="O43" t="s">
         <v>226</v>
-      </c>
-      <c r="O43" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
+        <v>72</v>
+      </c>
+      <c r="B44" t="s">
         <v>73</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
         <v>74</v>
-      </c>
-      <c r="C44" t="s">
-        <v>75</v>
       </c>
       <c r="D44" s="2">
         <v>44152</v>
@@ -3851,45 +3788,45 @@
         <v>44152</v>
       </c>
       <c r="F44" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G44" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H44">
         <v>1</v>
       </c>
       <c r="I44" t="s">
+        <v>228</v>
+      </c>
+      <c r="J44">
+        <v>23</v>
+      </c>
+      <c r="K44" t="s">
         <v>229</v>
       </c>
-      <c r="J44">
-        <v>23</v>
-      </c>
-      <c r="K44" t="s">
+      <c r="L44" t="s">
+        <v>228</v>
+      </c>
+      <c r="M44" t="s">
         <v>230</v>
       </c>
-      <c r="L44" t="s">
-        <v>229</v>
-      </c>
-      <c r="M44" t="s">
-        <v>231</v>
-      </c>
       <c r="N44" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="O44" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>37</v>
+      </c>
+      <c r="B45" t="s">
         <v>38</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
         <v>39</v>
-      </c>
-      <c r="C45" t="s">
-        <v>40</v>
       </c>
       <c r="D45" s="2">
         <v>44160</v>
@@ -3898,45 +3835,45 @@
         <v>44134</v>
       </c>
       <c r="F45" t="s">
+        <v>231</v>
+      </c>
+      <c r="G45" t="s">
         <v>232</v>
-      </c>
-      <c r="G45" t="s">
-        <v>233</v>
       </c>
       <c r="H45">
         <v>8.9512499999999999</v>
       </c>
       <c r="I45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J45">
         <v>23</v>
       </c>
       <c r="K45" t="s">
+        <v>233</v>
+      </c>
+      <c r="L45" t="s">
         <v>234</v>
       </c>
-      <c r="L45" t="s">
+      <c r="M45" t="s">
         <v>235</v>
       </c>
-      <c r="M45" t="s">
+      <c r="N45" t="s">
         <v>236</v>
       </c>
-      <c r="N45" t="s">
+      <c r="O45" t="s">
         <v>237</v>
-      </c>
-      <c r="O45" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>37</v>
+      </c>
+      <c r="B46" t="s">
         <v>38</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
         <v>39</v>
-      </c>
-      <c r="C46" t="s">
-        <v>40</v>
       </c>
       <c r="D46" s="2">
         <v>44160</v>
@@ -3945,45 +3882,45 @@
         <v>44134</v>
       </c>
       <c r="F46" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G46" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H46">
         <v>3.4175</v>
       </c>
       <c r="I46" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J46">
         <v>23</v>
       </c>
       <c r="K46" t="s">
+        <v>239</v>
+      </c>
+      <c r="L46" t="s">
         <v>240</v>
       </c>
-      <c r="L46" t="s">
+      <c r="M46" t="s">
         <v>241</v>
       </c>
-      <c r="M46" t="s">
-        <v>242</v>
-      </c>
       <c r="N46" t="s">
+        <v>236</v>
+      </c>
+      <c r="O46" t="s">
         <v>237</v>
-      </c>
-      <c r="O46" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>37</v>
+      </c>
+      <c r="B47" t="s">
         <v>38</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" t="s">
         <v>39</v>
-      </c>
-      <c r="C47" t="s">
-        <v>40</v>
       </c>
       <c r="D47" s="2">
         <v>44160</v>
@@ -3992,45 +3929,45 @@
         <v>44134</v>
       </c>
       <c r="F47" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G47" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H47">
         <v>14.5625</v>
       </c>
       <c r="I47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J47">
         <v>23</v>
       </c>
       <c r="K47" t="s">
+        <v>243</v>
+      </c>
+      <c r="L47" t="s">
         <v>244</v>
       </c>
-      <c r="L47" t="s">
+      <c r="M47" t="s">
         <v>245</v>
       </c>
-      <c r="M47" t="s">
-        <v>246</v>
-      </c>
       <c r="N47" t="s">
+        <v>236</v>
+      </c>
+      <c r="O47" t="s">
         <v>237</v>
-      </c>
-      <c r="O47" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>37</v>
+      </c>
+      <c r="B48" t="s">
         <v>38</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
         <v>39</v>
-      </c>
-      <c r="C48" t="s">
-        <v>40</v>
       </c>
       <c r="D48" s="2">
         <v>44160</v>
@@ -4039,45 +3976,45 @@
         <v>44134</v>
       </c>
       <c r="F48" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G48" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H48">
         <v>1.8125</v>
       </c>
       <c r="I48" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J48">
         <v>23</v>
       </c>
       <c r="K48" t="s">
+        <v>247</v>
+      </c>
+      <c r="L48" t="s">
         <v>248</v>
       </c>
-      <c r="L48" t="s">
+      <c r="M48" t="s">
         <v>249</v>
       </c>
-      <c r="M48" t="s">
-        <v>250</v>
-      </c>
       <c r="N48" t="s">
+        <v>236</v>
+      </c>
+      <c r="O48" t="s">
         <v>237</v>
-      </c>
-      <c r="O48" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
+        <v>37</v>
+      </c>
+      <c r="B49" t="s">
         <v>38</v>
       </c>
-      <c r="B49" t="s">
+      <c r="C49" t="s">
         <v>39</v>
-      </c>
-      <c r="C49" t="s">
-        <v>40</v>
       </c>
       <c r="D49" s="2">
         <v>44160</v>
@@ -4086,45 +4023,45 @@
         <v>44134</v>
       </c>
       <c r="F49" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G49" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H49">
         <v>0.5625</v>
       </c>
       <c r="I49" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J49">
         <v>23</v>
       </c>
       <c r="K49" t="s">
+        <v>251</v>
+      </c>
+      <c r="L49" t="s">
         <v>252</v>
       </c>
-      <c r="L49" t="s">
+      <c r="M49" t="s">
         <v>253</v>
       </c>
-      <c r="M49" t="s">
-        <v>254</v>
-      </c>
       <c r="N49" t="s">
+        <v>236</v>
+      </c>
+      <c r="O49" t="s">
         <v>237</v>
-      </c>
-      <c r="O49" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
+        <v>37</v>
+      </c>
+      <c r="B50" t="s">
         <v>38</v>
       </c>
-      <c r="B50" t="s">
+      <c r="C50" t="s">
         <v>39</v>
-      </c>
-      <c r="C50" t="s">
-        <v>40</v>
       </c>
       <c r="D50" s="2">
         <v>44160</v>
@@ -4133,45 +4070,45 @@
         <v>44134</v>
       </c>
       <c r="F50" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G50" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H50">
         <v>1.21875</v>
       </c>
       <c r="I50" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J50">
         <v>23</v>
       </c>
       <c r="K50" t="s">
+        <v>255</v>
+      </c>
+      <c r="L50" t="s">
         <v>256</v>
       </c>
-      <c r="L50" t="s">
+      <c r="M50" t="s">
         <v>257</v>
       </c>
-      <c r="M50" t="s">
-        <v>258</v>
-      </c>
       <c r="N50" t="s">
+        <v>236</v>
+      </c>
+      <c r="O50" t="s">
         <v>237</v>
-      </c>
-      <c r="O50" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>37</v>
+      </c>
+      <c r="B51" t="s">
         <v>38</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
         <v>39</v>
-      </c>
-      <c r="C51" t="s">
-        <v>40</v>
       </c>
       <c r="D51" s="2">
         <v>44160</v>
@@ -4180,45 +4117,45 @@
         <v>44134</v>
       </c>
       <c r="F51" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G51" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H51">
         <v>0.20624999999999999</v>
       </c>
       <c r="I51" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J51">
         <v>23</v>
       </c>
       <c r="K51" t="s">
+        <v>259</v>
+      </c>
+      <c r="L51" t="s">
         <v>260</v>
       </c>
-      <c r="L51" t="s">
+      <c r="M51" t="s">
         <v>261</v>
       </c>
-      <c r="M51" t="s">
-        <v>262</v>
-      </c>
       <c r="N51" t="s">
+        <v>236</v>
+      </c>
+      <c r="O51" t="s">
         <v>237</v>
-      </c>
-      <c r="O51" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>37</v>
+      </c>
+      <c r="B52" t="s">
         <v>38</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C52" t="s">
         <v>39</v>
-      </c>
-      <c r="C52" t="s">
-        <v>40</v>
       </c>
       <c r="D52" s="2">
         <v>44160</v>
@@ -4227,45 +4164,45 @@
         <v>44134</v>
       </c>
       <c r="F52" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G52" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H52">
         <v>3.2987500000000001</v>
       </c>
       <c r="I52" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J52">
         <v>23</v>
       </c>
       <c r="K52" t="s">
+        <v>263</v>
+      </c>
+      <c r="L52" t="s">
         <v>264</v>
       </c>
-      <c r="L52" t="s">
+      <c r="M52" t="s">
         <v>265</v>
       </c>
-      <c r="M52" t="s">
-        <v>266</v>
-      </c>
       <c r="N52" t="s">
+        <v>236</v>
+      </c>
+      <c r="O52" t="s">
         <v>237</v>
-      </c>
-      <c r="O52" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
+        <v>37</v>
+      </c>
+      <c r="B53" t="s">
         <v>38</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C53" t="s">
         <v>39</v>
-      </c>
-      <c r="C53" t="s">
-        <v>40</v>
       </c>
       <c r="D53" s="2">
         <v>44160</v>
@@ -4274,45 +4211,45 @@
         <v>44134</v>
       </c>
       <c r="F53" t="s">
+        <v>266</v>
+      </c>
+      <c r="G53" t="s">
         <v>267</v>
-      </c>
-      <c r="G53" t="s">
-        <v>268</v>
       </c>
       <c r="H53">
         <v>12.775</v>
       </c>
       <c r="I53" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J53">
         <v>23</v>
       </c>
       <c r="K53" t="s">
+        <v>268</v>
+      </c>
+      <c r="L53" t="s">
         <v>269</v>
       </c>
-      <c r="L53" t="s">
+      <c r="M53" t="s">
         <v>270</v>
       </c>
-      <c r="M53" t="s">
-        <v>271</v>
-      </c>
       <c r="N53" t="s">
+        <v>269</v>
+      </c>
+      <c r="O53" t="s">
         <v>270</v>
-      </c>
-      <c r="O53" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
+        <v>37</v>
+      </c>
+      <c r="B54" t="s">
         <v>38</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" t="s">
         <v>39</v>
-      </c>
-      <c r="C54" t="s">
-        <v>40</v>
       </c>
       <c r="D54" s="2">
         <v>44160</v>
@@ -4321,45 +4258,45 @@
         <v>44160</v>
       </c>
       <c r="F54" t="s">
+        <v>271</v>
+      </c>
+      <c r="G54" t="s">
         <v>272</v>
-      </c>
-      <c r="G54" t="s">
-        <v>273</v>
       </c>
       <c r="H54">
         <v>18.25</v>
       </c>
       <c r="I54" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J54">
         <v>23</v>
       </c>
       <c r="K54" t="s">
+        <v>273</v>
+      </c>
+      <c r="L54" t="s">
         <v>274</v>
       </c>
-      <c r="L54" t="s">
+      <c r="M54" t="s">
         <v>275</v>
       </c>
-      <c r="M54" t="s">
+      <c r="N54" t="s">
         <v>276</v>
       </c>
-      <c r="N54" t="s">
+      <c r="O54" t="s">
         <v>277</v>
-      </c>
-      <c r="O54" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
+        <v>37</v>
+      </c>
+      <c r="B55" t="s">
         <v>38</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
         <v>39</v>
-      </c>
-      <c r="C55" t="s">
-        <v>40</v>
       </c>
       <c r="D55" s="2">
         <v>44160</v>
@@ -4368,45 +4305,45 @@
         <v>44160</v>
       </c>
       <c r="F55" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G55" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H55">
         <v>2.5</v>
       </c>
       <c r="I55" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J55">
         <v>23</v>
       </c>
       <c r="K55" t="s">
+        <v>279</v>
+      </c>
+      <c r="L55" t="s">
+        <v>117</v>
+      </c>
+      <c r="M55" t="s">
         <v>280</v>
       </c>
-      <c r="L55" t="s">
-        <v>118</v>
-      </c>
-      <c r="M55" t="s">
-        <v>281</v>
-      </c>
       <c r="N55" t="s">
+        <v>276</v>
+      </c>
+      <c r="O55" t="s">
         <v>277</v>
-      </c>
-      <c r="O55" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>37</v>
+      </c>
+      <c r="B56" t="s">
         <v>38</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" t="s">
         <v>39</v>
-      </c>
-      <c r="C56" t="s">
-        <v>40</v>
       </c>
       <c r="D56" s="2">
         <v>44160</v>
@@ -4415,45 +4352,45 @@
         <v>44160</v>
       </c>
       <c r="F56" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G56" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H56">
         <v>3</v>
       </c>
       <c r="I56" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J56">
         <v>23</v>
       </c>
       <c r="K56" t="s">
+        <v>21</v>
+      </c>
+      <c r="L56" t="s">
+        <v>20</v>
+      </c>
+      <c r="M56" t="s">
         <v>22</v>
       </c>
-      <c r="L56" t="s">
-        <v>21</v>
-      </c>
-      <c r="M56" t="s">
-        <v>23</v>
-      </c>
       <c r="N56" t="s">
+        <v>276</v>
+      </c>
+      <c r="O56" t="s">
         <v>277</v>
-      </c>
-      <c r="O56" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
+        <v>37</v>
+      </c>
+      <c r="B57" t="s">
         <v>38</v>
       </c>
-      <c r="B57" t="s">
+      <c r="C57" t="s">
         <v>39</v>
-      </c>
-      <c r="C57" t="s">
-        <v>40</v>
       </c>
       <c r="D57" s="2">
         <v>44160</v>
@@ -4462,16 +4399,14 @@
         <v>44160</v>
       </c>
       <c r="F57" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G57" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="A59" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
skończone parsery dzialaja cudownie
</commit_message>
<xml_diff>
--- a/zadanie3/faktury-sprzedazowe-test.xlsx
+++ b/zadanie3/faktury-sprzedazowe-test.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FiFi\PZ1\zadanie3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D92908F-FB8F-4933-A75E-D3B1860B3E9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E81086-4274-4040-B496-3106A1C6F085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15870" yWindow="270" windowWidth="15990" windowHeight="24840"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="faktury-sprzedazowe-test" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="282">
   <si>
     <t>Nazwa odbiorcy</t>
   </si>
@@ -866,15 +866,12 @@
   </si>
   <si>
     <t xml:space="preserve">Prace rozwojowe - #69169 :PodziaĹ‚ ruchu na iframe/zalogowany/anonimowy </t>
-  </si>
-  <si>
-    <t>Prace rozwojowe - #69401 : Dodatki po audycie UX</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1730,11 +1727,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4383,27 +4380,8 @@
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>37</v>
-      </c>
-      <c r="B57" t="s">
-        <v>38</v>
-      </c>
-      <c r="C57" t="s">
-        <v>39</v>
-      </c>
-      <c r="D57" s="2">
-        <v>44160</v>
-      </c>
-      <c r="E57" s="2">
-        <v>44160</v>
-      </c>
-      <c r="F57" t="s">
-        <v>271</v>
-      </c>
-      <c r="G57" t="s">
-        <v>282</v>
-      </c>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>

</xml_diff>